<commit_message>
Code Cleared, add dots to banner, addproduct feature bugs resolved
</commit_message>
<xml_diff>
--- a/src/assets/ExcelSampleFile/Categories_Sample.xlsx
+++ b/src/assets/ExcelSampleFile/Categories_Sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\OneDrive\Desktop\Venture Pact\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tradevogue\eCommerce-frontend\src\assets\ExcelSampleFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F75C5D3-D66D-4E59-870F-201179A4BACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE96B29A-8541-4D6A-8FE0-1FAA3EAF700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Category 1</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Category 7</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -369,49 +369,49 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>